<commit_message>
Sprint review, daily standup, updated sprint info
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint5.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint5.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -477,10 +477,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -974,31 +974,31 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>53</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2304,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,10 +2408,10 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -2448,8 +2448,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="15" t="s">
         <v>49</v>
       </c>
@@ -2468,7 +2468,9 @@
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="M6" s="15">
+        <v>4</v>
+      </c>
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
       <c r="P6" s="15"/>
@@ -2478,12 +2480,12 @@
       <c r="T6" s="15"/>
       <c r="U6" s="15">
         <f>E6-SUM(G6:T6)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="15" t="s">
         <v>50</v>
       </c>
@@ -2502,7 +2504,9 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
+      <c r="M7" s="15">
+        <v>10</v>
+      </c>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
@@ -2512,12 +2516,12 @@
       <c r="T7" s="15"/>
       <c r="U7" s="15">
         <f t="shared" ref="U7:U25" si="0">E7-SUM(G7:T7)</f>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="15" t="s">
         <v>52</v>
       </c>
@@ -2548,8 +2552,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="15" t="s">
         <v>51</v>
       </c>
@@ -2578,7 +2582,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="27">
@@ -2593,13 +2597,17 @@
       <c r="E10" s="15">
         <v>3</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="L10" s="15">
+        <v>3</v>
+      </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
@@ -2610,11 +2618,11 @@
       <c r="T10" s="15"/>
       <c r="U10" s="15">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="28"/>
       <c r="C11" s="15" t="s">
         <v>46</v>
@@ -2625,7 +2633,9 @@
       <c r="E11" s="15">
         <v>2</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -2646,7 +2656,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="29"/>
       <c r="C12" s="15" t="s">
         <v>47</v>
@@ -2676,7 +2686,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="27">
@@ -2710,7 +2720,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="28"/>
       <c r="C14" s="15" t="s">
         <v>46</v>
@@ -2740,7 +2750,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="29"/>
       <c r="C15" s="15" t="s">
         <v>47</v>
@@ -2770,7 +2780,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="27">
@@ -2785,14 +2795,18 @@
       <c r="E16" s="15">
         <v>2</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
+      <c r="M16" s="15">
+        <v>2</v>
+      </c>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
@@ -2802,11 +2816,11 @@
       <c r="T16" s="15"/>
       <c r="U16" s="15">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="28"/>
       <c r="C17" s="15" t="s">
         <v>46</v>
@@ -2817,7 +2831,9 @@
       <c r="E17" s="15">
         <v>1</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -2838,7 +2854,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="29"/>
       <c r="C18" s="15" t="s">
         <v>47</v>
@@ -2868,7 +2884,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="26" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="27">
@@ -2902,7 +2918,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="28"/>
       <c r="C20" s="15" t="s">
         <v>46</v>
@@ -2932,7 +2948,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="29"/>
       <c r="C21" s="15" t="s">
         <v>47</v>
@@ -2962,7 +2978,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="26" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="27">
@@ -2977,14 +2993,18 @@
       <c r="E22" s="15">
         <v>1</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
+      <c r="M22" s="15">
+        <v>1</v>
+      </c>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
@@ -2994,11 +3014,11 @@
       <c r="T22" s="15"/>
       <c r="U22" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="28"/>
       <c r="C23" s="15" t="s">
         <v>46</v>
@@ -3030,7 +3050,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="29"/>
       <c r="C24" s="15" t="s">
         <v>47</v>
@@ -3096,11 +3116,11 @@
       </c>
       <c r="L25" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M25" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N25" s="15">
         <f t="shared" si="3"/>
@@ -3132,7 +3152,7 @@
       </c>
       <c r="U25" s="15">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3239,39 +3259,39 @@
       </c>
       <c r="L27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="N27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="O27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="P27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="Q27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="R27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="S27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="T27" s="15">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="U27" s="17"/>
     </row>
@@ -3307,18 +3327,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F12">
     <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">

</xml_diff>

<commit_message>
Added task for Gui implementation
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint5.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint5.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\MasterAudioTechnologyFunctions\Documentation and designs\Sprint_info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djnenadovic\Desktop\MATF\MasterAudioTechnologyFunctions\Documentation and designs\Sprint_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sprint" sheetId="1" r:id="rId2"/>
     <sheet name="Chart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -211,12 +211,15 @@
   </si>
   <si>
     <t>To do</t>
+  </si>
+  <si>
+    <t>Deploy to feature</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -429,7 +432,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
@@ -476,6 +479,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,10 +501,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -516,7 +522,7 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="18">
     <dxf>
       <font>
         <color theme="0"/>
@@ -579,21 +585,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -626,21 +617,6 @@
           <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -681,7 +657,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -726,6 +702,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -757,7 +734,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sr-Latn-RS"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -772,7 +749,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint!$E$29</c:f>
+              <c:f>Sprint!$E$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -851,60 +828,60 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint!$F$29:$T$29</c:f>
+              <c:f>Sprint!$F$30:$T$30</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>64</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.428571428571431</c:v>
+                  <c:v>62.214285714285715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.857142857142861</c:v>
+                  <c:v>57.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.285714285714292</c:v>
+                  <c:v>52.642857142857146</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.714285714285722</c:v>
+                  <c:v>47.857142857142861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.142857142857153</c:v>
+                  <c:v>43.071428571428577</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.571428571428584</c:v>
+                  <c:v>38.285714285714292</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.000000000000014</c:v>
+                  <c:v>33.500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.428571428571445</c:v>
+                  <c:v>28.714285714285722</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.857142857142875</c:v>
+                  <c:v>23.928571428571438</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18.285714285714306</c:v>
+                  <c:v>19.142857142857153</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.714285714285735</c:v>
+                  <c:v>14.357142857142868</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.1428571428571637</c:v>
+                  <c:v>9.5714285714285836</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.5714285714285925</c:v>
+                  <c:v>4.785714285714298</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1316282072803006E-14</c:v>
+                  <c:v>1.2434497875801753E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2B6F-4357-9072-E062BD4EF823}"/>
             </c:ext>
@@ -915,7 +892,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint!$E$30</c:f>
+              <c:f>Sprint!$E$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -994,60 +971,60 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint!$F$30:$T$30</c:f>
+              <c:f>Sprint!$F$31:$T$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>58</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>41</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2B6F-4357-9072-E062BD4EF823}"/>
             </c:ext>
@@ -1062,11 +1039,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="308619040"/>
-        <c:axId val="308624616"/>
+        <c:axId val="321810624"/>
+        <c:axId val="321815720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="308619040"/>
+        <c:axId val="321810624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1106,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="sr-Latn-RS"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1166,10 +1143,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sr-Latn-RS"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308624616"/>
+        <c:crossAx val="321815720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1177,7 +1154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="308624616"/>
+        <c:axId val="321815720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1222,6 +1199,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1246,7 +1224,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="sr-Latn-RS"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1277,10 +1255,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sr-Latn-RS"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308619040"/>
+        <c:crossAx val="321810624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1328,7 +1306,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sr-Latn-RS"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1376,7 +1354,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sr-Latn-RS"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1943,7 +1921,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2276,21 +2254,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2299,10 +2277,10 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2311,10 +2289,10 @@
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2323,10 +2301,10 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
@@ -2345,10 +2323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,7 +2432,7 @@
       <c r="A5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="28">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -2492,7 +2470,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="26"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="15" t="s">
         <v>49</v>
       </c>
@@ -2529,8 +2507,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="15" t="s">
         <v>50</v>
       </c>
@@ -2562,13 +2540,13 @@
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
       <c r="U7" s="15">
-        <f t="shared" ref="U7:U28" si="0">E7-SUM(G7:T7)</f>
+        <f t="shared" ref="U7:U29" si="0">E7-SUM(G7:T7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="15" t="s">
         <v>52</v>
       </c>
@@ -2601,66 +2579,60 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="15" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="20">
+        <v>3</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20">
+        <f>E9-SUM(G9:T9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E10" s="15">
         <v>2</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="28">
-        <v>5</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="15">
-        <v>3</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>53</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="15">
-        <v>3</v>
-      </c>
+      <c r="L10" s="15"/>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
@@ -2671,30 +2643,36 @@
       <c r="T10" s="15"/>
       <c r="U10" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="29">
+        <v>5</v>
+      </c>
       <c r="C11" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="L11" s="15">
+        <v>3</v>
+      </c>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
@@ -2705,21 +2683,23 @@
       <c r="T11" s="15"/>
       <c r="U11" s="15">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="30"/>
       <c r="C12" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="15"/>
+        <v>46</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="E12" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -2737,24 +2717,20 @@
       <c r="T12" s="15"/>
       <c r="U12" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="28">
-        <v>8</v>
-      </c>
+      <c r="A13" s="28"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15">
-        <v>5</v>
-      </c>
-      <c r="F13" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>59</v>
       </c>
       <c r="G13" s="15"/>
@@ -2772,15 +2748,19 @@
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
       <c r="U13" s="15">
-        <f t="shared" ref="U13:U18" si="1">E13-SUM(G13:T13)</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="29">
+        <v>8</v>
+      </c>
       <c r="C14" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15">
@@ -2804,19 +2784,19 @@
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
       <c r="U14" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="U14:U19" si="1">E14-SUM(G14:T14)</f>
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="30"/>
       <c r="C15" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>59</v>
@@ -2837,27 +2817,21 @@
       <c r="T15" s="15"/>
       <c r="U15" s="15">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="28">
-        <v>3</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="15">
-        <v>2</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>53</v>
+      <c r="F16" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -2865,9 +2839,7 @@
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="15">
-        <v>2</v>
-      </c>
+      <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
@@ -2877,23 +2849,27 @@
       <c r="T16" s="15"/>
       <c r="U16" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="29">
+        <v>3</v>
+      </c>
       <c r="C17" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
@@ -2901,7 +2877,9 @@
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
+      <c r="M17" s="15">
+        <v>2</v>
+      </c>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
@@ -2911,21 +2889,23 @@
       <c r="T17" s="15"/>
       <c r="U17" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="30"/>
       <c r="C18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="15"/>
+        <v>46</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E18" s="15">
         <v>1</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -2947,20 +2927,16 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="28">
-        <v>8</v>
-      </c>
+      <c r="A19" s="28"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15">
-        <v>5</v>
-      </c>
-      <c r="F19" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>59</v>
       </c>
       <c r="G19" s="15"/>
@@ -2978,19 +2954,23 @@
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
       <c r="U19" s="15">
-        <f t="shared" ref="U19:U24" si="2">E19-SUM(G19:T19)</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="29">
+        <v>8</v>
+      </c>
       <c r="C20" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>59</v>
@@ -3010,19 +2990,19 @@
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
       <c r="U20" s="15">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" ref="U20:U25" si="2">E20-SUM(G20:T20)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="30"/>
       <c r="C21" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="19" t="s">
         <v>59</v>
@@ -3043,27 +3023,21 @@
       <c r="T21" s="15"/>
       <c r="U21" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="28">
-        <v>3</v>
-      </c>
+      <c r="A22" s="28"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>6</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D22" s="15"/>
       <c r="E22" s="15">
         <v>1</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>53</v>
+      <c r="F22" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -3071,9 +3045,7 @@
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
-      <c r="M22" s="15">
-        <v>1</v>
-      </c>
+      <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
@@ -3083,14 +3055,18 @@
       <c r="T22" s="15"/>
       <c r="U22" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="29">
+        <v>3</v>
+      </c>
       <c r="C23" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>6</v>
@@ -3099,7 +3075,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -3107,7 +3083,9 @@
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
+      <c r="M23" s="15">
+        <v>1</v>
+      </c>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
@@ -3117,20 +3095,22 @@
       <c r="T23" s="15"/>
       <c r="U23" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="30"/>
       <c r="C24" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="15"/>
+        <v>46</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E24" s="15">
         <v>1</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="15" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="15"/>
@@ -3153,56 +3133,52 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="28"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="28">
+      <c r="B26" s="29">
         <v>8</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="19">
-        <v>5</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19">
-        <v>5</v>
-      </c>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19">
-        <f t="shared" ref="U25:U27" si="3">E25-SUM(G25:T25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>53</v>
@@ -3215,7 +3191,7 @@
       <c r="L26" s="19"/>
       <c r="M26" s="19"/>
       <c r="N26" s="19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
@@ -3224,22 +3200,24 @@
       <c r="S26" s="19"/>
       <c r="T26" s="19"/>
       <c r="U26" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="U26:U28" si="3">E26-SUM(G26:T26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="30"/>
       <c r="C27" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="19"/>
+        <v>57</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E27" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
@@ -3248,7 +3226,9 @@
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
+      <c r="N27" s="19">
+        <v>2</v>
+      </c>
       <c r="O27" s="19"/>
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
@@ -3257,154 +3237,116 @@
       <c r="T27" s="19"/>
       <c r="U27" s="19">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="F28" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="15">
-        <f>SUM(B5:B27)</f>
+      <c r="B29" s="15">
+        <f>SUM(B5:B28)</f>
         <v>55</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="15">
-        <f>SUM(E5:E27)</f>
-        <v>64</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="15">
-        <f>SUM(G5:G27)</f>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="15">
+        <f>SUM(E5:E28)</f>
+        <v>67</v>
+      </c>
+      <c r="F29" s="16"/>
+      <c r="G29" s="15">
+        <f>SUM(G5:G28)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="15">
-        <f>SUM(H5:H27)</f>
+      <c r="H29" s="15">
+        <f>SUM(H5:H28)</f>
         <v>3</v>
       </c>
-      <c r="I28" s="19">
-        <f t="shared" ref="I28:T28" si="4">SUM(I5:I27)</f>
+      <c r="I29" s="19">
+        <f t="shared" ref="I29:T29" si="4">SUM(I5:I28)</f>
         <v>0</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L28" s="19">
+      <c r="L29" s="19">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="M28" s="19">
+      <c r="M29" s="19">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="N28" s="19">
+      <c r="N29" s="19">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="O28" s="19">
+      <c r="O29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="Q29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R28" s="19">
+      <c r="R29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S28" s="19">
+      <c r="S29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T28" s="19">
+      <c r="T29" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U28" s="15">
+      <c r="U29" s="15">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="15">
-        <f>SUM(E5:E27)</f>
-        <v>64</v>
-      </c>
-      <c r="G29" s="18">
-        <f>F29-F29/14</f>
-        <v>59.428571428571431</v>
-      </c>
-      <c r="H29" s="18">
-        <f>G29-F29/14</f>
-        <v>54.857142857142861</v>
-      </c>
-      <c r="I29" s="18">
-        <f>H29-F29/14</f>
-        <v>50.285714285714292</v>
-      </c>
-      <c r="J29" s="18">
-        <f>I29-F29/14</f>
-        <v>45.714285714285722</v>
-      </c>
-      <c r="K29" s="18">
-        <f>J29-F29/14</f>
-        <v>41.142857142857153</v>
-      </c>
-      <c r="L29" s="18">
-        <f>K29-F29/14</f>
-        <v>36.571428571428584</v>
-      </c>
-      <c r="M29" s="18">
-        <f>L29-F29/14</f>
-        <v>32.000000000000014</v>
-      </c>
-      <c r="N29" s="18">
-        <f>M29-F29/14</f>
-        <v>27.428571428571445</v>
-      </c>
-      <c r="O29" s="18">
-        <f>N29-F29/14</f>
-        <v>22.857142857142875</v>
-      </c>
-      <c r="P29" s="18">
-        <f>O29-F29/14</f>
-        <v>18.285714285714306</v>
-      </c>
-      <c r="Q29" s="18">
-        <f>P29-F29/14</f>
-        <v>13.714285714285735</v>
-      </c>
-      <c r="R29" s="18">
-        <f>Q29-F29/14</f>
-        <v>9.1428571428571637</v>
-      </c>
-      <c r="S29" s="18">
-        <f>R29-F29/14</f>
-        <v>4.5714285714285925</v>
-      </c>
-      <c r="T29" s="18">
-        <f>S29-F29/14</f>
-        <v>2.1316282072803006E-14</v>
-      </c>
-      <c r="U29" s="17"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
@@ -3412,75 +3354,139 @@
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="15">
+        <f>SUM(E5:E28)</f>
+        <v>67</v>
+      </c>
+      <c r="G30" s="18">
+        <f>F30-F30/14</f>
+        <v>62.214285714285715</v>
+      </c>
+      <c r="H30" s="18">
+        <f>G30-F30/14</f>
+        <v>57.428571428571431</v>
+      </c>
+      <c r="I30" s="18">
+        <f>H30-F30/14</f>
+        <v>52.642857142857146</v>
+      </c>
+      <c r="J30" s="18">
+        <f>I30-F30/14</f>
+        <v>47.857142857142861</v>
+      </c>
+      <c r="K30" s="18">
+        <f>J30-F30/14</f>
+        <v>43.071428571428577</v>
+      </c>
+      <c r="L30" s="18">
+        <f>K30-F30/14</f>
+        <v>38.285714285714292</v>
+      </c>
+      <c r="M30" s="18">
+        <f>L30-F30/14</f>
+        <v>33.500000000000007</v>
+      </c>
+      <c r="N30" s="18">
+        <f>M30-F30/14</f>
+        <v>28.714285714285722</v>
+      </c>
+      <c r="O30" s="18">
+        <f>N30-F30/14</f>
+        <v>23.928571428571438</v>
+      </c>
+      <c r="P30" s="18">
+        <f>O30-F30/14</f>
+        <v>19.142857142857153</v>
+      </c>
+      <c r="Q30" s="18">
+        <f>P30-F30/14</f>
+        <v>14.357142857142868</v>
+      </c>
+      <c r="R30" s="18">
+        <f>Q30-F30/14</f>
+        <v>9.5714285714285836</v>
+      </c>
+      <c r="S30" s="18">
+        <f>R30-F30/14</f>
+        <v>4.785714285714298</v>
+      </c>
+      <c r="T30" s="18">
+        <f>S30-F30/14</f>
+        <v>1.2434497875801753E-14</v>
+      </c>
+      <c r="U30" s="17"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="15">
-        <f>SUM(E5:E27)</f>
+      <c r="F31" s="15">
+        <f>SUM(E5:E28)</f>
+        <v>67</v>
+      </c>
+      <c r="G31" s="15">
+        <f>F31-SUM(G5:G28)</f>
+        <v>67</v>
+      </c>
+      <c r="H31" s="15">
+        <f>G31-SUM(H5:H28)</f>
         <v>64</v>
       </c>
-      <c r="G30" s="15">
-        <f>F30-SUM(G5:G27)</f>
+      <c r="I31" s="19">
+        <f t="shared" ref="I31:T31" si="5">H31-SUM(I5:I28)</f>
         <v>64</v>
       </c>
-      <c r="H30" s="15">
-        <f>G30-SUM(H5:H27)</f>
-        <v>61</v>
-      </c>
-      <c r="I30" s="19">
-        <f t="shared" ref="I30:T30" si="5">H30-SUM(I5:I27)</f>
-        <v>61</v>
-      </c>
-      <c r="J30" s="19">
+      <c r="J31" s="19">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="K31" s="19">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="L31" s="19">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
-      <c r="K30" s="19">
+      <c r="M31" s="19">
         <f t="shared" si="5"/>
-        <v>61</v>
-      </c>
-      <c r="L30" s="19">
+        <v>44</v>
+      </c>
+      <c r="N31" s="19">
         <f t="shared" si="5"/>
-        <v>58</v>
-      </c>
-      <c r="M30" s="19">
+        <v>33</v>
+      </c>
+      <c r="O31" s="19">
         <f t="shared" si="5"/>
-        <v>41</v>
-      </c>
-      <c r="N30" s="19">
+        <v>33</v>
+      </c>
+      <c r="P31" s="19">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="O30" s="19">
+        <v>33</v>
+      </c>
+      <c r="Q31" s="19">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="P30" s="19">
+        <v>33</v>
+      </c>
+      <c r="R31" s="19">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="Q30" s="19">
+        <v>33</v>
+      </c>
+      <c r="S31" s="19">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="R30" s="19">
+        <v>33</v>
+      </c>
+      <c r="T31" s="19">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="S30" s="19">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="T30" s="19">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="U30" s="17"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
+        <v>33</v>
+      </c>
+      <c r="U31" s="17"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
@@ -3506,66 +3512,72 @@
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F15">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+  <conditionalFormatting sqref="F5:F16">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="26" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U28 U5:U12">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
+  <conditionalFormatting sqref="U29 U5:U13">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U13:U15">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
+  <conditionalFormatting sqref="U14:U16">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:F21">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+  <conditionalFormatting sqref="F17:F22">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U16:U18">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="U17:U19">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U19:U21">
+  <conditionalFormatting sqref="U20:U22">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F24">
+  <conditionalFormatting sqref="F23:F25">
     <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -3576,12 +3588,12 @@
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U22:U24">
+  <conditionalFormatting sqref="U23:U25">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F27">
+  <conditionalFormatting sqref="F26:F28">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -3592,13 +3604,13 @@
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U25:U27">
+  <conditionalFormatting sqref="U26:U28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="491" yWindow="329" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F28">
       <formula1>"To do, In progress, Done"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3611,7 +3623,7 @@
           <x14:formula1>
             <xm:f>Roster!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D27</xm:sqref>
+          <xm:sqref>D5:D28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added latest user stories
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint5.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint5.xlsx
@@ -183,9 +183,6 @@
     <t>Implement already designed GUI elements</t>
   </si>
   <si>
-    <t>Implement already implemented functionalities</t>
-  </si>
-  <si>
     <t>Test for eventual bugs</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>To do</t>
+  </si>
+  <si>
+    <t>Reimplement functionalities</t>
   </si>
 </sst>
 </file>
@@ -495,10 +495,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1002,16 +1002,16 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2317,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2421,10 +2421,10 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="27">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -2437,7 +2437,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15">
@@ -2461,8 +2461,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="15" t="s">
         <v>49</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -2499,10 +2499,10 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="15" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>9</v>
@@ -2511,7 +2511,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -2537,10 +2537,10 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>3</v>
@@ -2549,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
@@ -2573,10 +2573,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>9</v>
@@ -2585,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -2597,17 +2597,19 @@
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
+      <c r="Q9" s="15">
+        <v>2</v>
+      </c>
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
       <c r="U9" s="15">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="28">
@@ -2623,7 +2625,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
@@ -2647,7 +2649,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="29"/>
       <c r="C11" s="15" t="s">
         <v>46</v>
@@ -2659,7 +2661,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -2681,7 +2683,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="30"/>
       <c r="C12" s="15" t="s">
         <v>47</v>
@@ -2691,7 +2693,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -2713,7 +2715,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="28">
@@ -2727,7 +2729,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -2749,7 +2751,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="29"/>
       <c r="C14" s="15" t="s">
         <v>46</v>
@@ -2759,7 +2761,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -2781,7 +2783,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="30"/>
       <c r="C15" s="15" t="s">
         <v>47</v>
@@ -2791,7 +2793,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -2813,7 +2815,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="28">
@@ -2829,7 +2831,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -2853,7 +2855,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="29"/>
       <c r="C17" s="15" t="s">
         <v>46</v>
@@ -2865,7 +2867,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
@@ -2887,7 +2889,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="30"/>
       <c r="C18" s="15" t="s">
         <v>47</v>
@@ -2897,7 +2899,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -2919,7 +2921,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="28">
@@ -2933,7 +2935,7 @@
         <v>5</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -2955,7 +2957,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="29"/>
       <c r="C20" s="15" t="s">
         <v>46</v>
@@ -2965,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -2987,7 +2989,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="30"/>
       <c r="C21" s="15" t="s">
         <v>47</v>
@@ -2997,7 +2999,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
@@ -3019,7 +3021,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="28">
@@ -3035,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -3059,7 +3061,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="29"/>
       <c r="C23" s="15" t="s">
         <v>46</v>
@@ -3071,7 +3073,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -3093,7 +3095,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="30"/>
       <c r="C24" s="15" t="s">
         <v>47</v>
@@ -3103,7 +3105,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -3125,14 +3127,14 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>55</v>
+      <c r="A25" s="26" t="s">
+        <v>54</v>
       </c>
       <c r="B25" s="28">
         <v>8</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>9</v>
@@ -3141,7 +3143,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
@@ -3165,10 +3167,10 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="29"/>
       <c r="C26" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>9</v>
@@ -3177,7 +3179,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
@@ -3201,10 +3203,10 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="30"/>
       <c r="C27" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>3</v>
@@ -3213,7 +3215,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
@@ -3293,7 +3295,7 @@
       </c>
       <c r="Q28" s="19">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R28" s="19">
         <f t="shared" si="4"/>
@@ -3309,7 +3311,7 @@
       </c>
       <c r="U28" s="15">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -3436,19 +3438,19 @@
       </c>
       <c r="Q30" s="19">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R30" s="19">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S30" s="19">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="T30" s="19">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="U30" s="17"/>
     </row>
@@ -3484,6 +3486,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="A16:A18"/>
@@ -3492,12 +3500,6 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F15">
     <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">

</xml_diff>